<commit_message>
fill in A-10 report readme for new checks
</commit_message>
<xml_diff>
--- a/validation_tool/reports/a10_facility_check_report.xlsx
+++ b/validation_tool/reports/a10_facility_check_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="224">
   <si>
     <t>Organization</t>
   </si>
@@ -662,7 +662,10 @@
     <t>Read Me</t>
   </si>
   <si>
-    <t>This file runs 3 validation checks on submitted 2023-A-10 form data, based on historical NTD validation errors.</t>
+    <t>This file runs 6 validation checks on submitted 2023-A-10 form data, based on historical NTD validation errors.</t>
+  </si>
+  <si>
+    <t>Total Facilities checks</t>
   </si>
   <si>
     <t>1. "Whole Number Facilities": Check that sum of total facilities for each agency, across all modes, is a whole number.</t>
@@ -671,7 +674,19 @@
     <t>2. "Non-zero Facilities" check: Check that the sum of all total facilities is not zero.</t>
   </si>
   <si>
-    <t>3. "General Purpose Facility check": Check whether total gen purpose facilities (all but heavy maintenance) is &gt; 1. If so mark as "failure".</t>
+    <t>General Purpose Facilities checks (all except "heavy maintenance")</t>
+  </si>
+  <si>
+    <t>3. "Gen  Purpose Facilities": Check whether total gen purpose facilities (all but heavy maintenance) is &gt; 1. If so mark as "failure".</t>
+  </si>
+  <si>
+    <t>4. "Multiple Gen Purpose Facilities": if &gt; 1 reported, ask for narrative justification.</t>
+  </si>
+  <si>
+    <t>5. "Comparison to last yr: Gen Purpose Facilities": Fail if the total differs from last year</t>
+  </si>
+  <si>
+    <t>6. "Non-zero Gen Purpose Facilities": fail if this is reported as 0</t>
   </si>
 </sst>
 </file>
@@ -8521,7 +8536,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8537,19 +8552,44 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>